<commit_message>
GoodInfo_v2 - 2021.11.19 raw data
</commit_message>
<xml_diff>
--- a/GoodInfo_StockList_20211118.xlsx
+++ b/GoodInfo_StockList_20211118.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ray\Documents\Python\GoodInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RayWu\OneDrive - AAEON Technology\_OLD\Documents\Python\TradingModel_GoodInfo_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_954F2878EEF234A9C0B006BA18E0511D32EF47D8" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1DBA6E64-D380-4CC7-BD25-CB1228C4156D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="7440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="7440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>名稱</t>
   </si>
@@ -286,25 +287,13 @@
   </si>
   <si>
     <t>大量_小計</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -683,25 +672,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="8.5" customWidth="1"/>
-    <col min="7" max="7" width="8.625" customWidth="1"/>
-    <col min="8" max="8" width="8.25" customWidth="1"/>
-    <col min="9" max="9" width="8.875" customWidth="1"/>
-    <col min="10" max="10" width="10.25" customWidth="1"/>
-    <col min="11" max="11" width="10.5" customWidth="1"/>
-    <col min="12" max="12" width="9.875" customWidth="1"/>
+    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="8.625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.25" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="8.875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10.25" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>79</v>
       </c>
@@ -754,7 +745,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>38</v>
       </c>
@@ -801,11 +792,11 @@
         <v>3.12</v>
       </c>
       <c r="R2">
-        <f>O2+P2+Q2</f>
+        <f t="shared" ref="R2:R33" si="0">O2+P2+Q2</f>
         <v>3.12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>14</v>
       </c>
@@ -852,11 +843,11 @@
         <v>3.37</v>
       </c>
       <c r="R3">
-        <f>O3+P3+Q3</f>
+        <f t="shared" si="0"/>
         <v>3.37</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>63</v>
       </c>
@@ -906,11 +897,11 @@
         <v>10.01</v>
       </c>
       <c r="R4">
-        <f>O4+P4+Q4</f>
+        <f t="shared" si="0"/>
         <v>14.69</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>51</v>
       </c>
@@ -957,14 +948,11 @@
         <v>0.7</v>
       </c>
       <c r="R5">
-        <f>O5+P5+Q5</f>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="S5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>34</v>
       </c>
@@ -1011,14 +999,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="R6">
-        <f>O6+P6+Q6</f>
+        <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="S6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>55</v>
       </c>
@@ -1065,14 +1050,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="R7">
-        <f>O7+P7+Q7</f>
+        <f t="shared" si="0"/>
         <v>2.2999999999999998</v>
       </c>
-      <c r="S7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>39</v>
       </c>
@@ -1119,14 +1101,11 @@
         <v>3.45</v>
       </c>
       <c r="R8">
-        <f>O8+P8+Q8</f>
+        <f t="shared" si="0"/>
         <v>3.45</v>
       </c>
-      <c r="S8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>37</v>
       </c>
@@ -1173,14 +1152,11 @@
         <v>3.65</v>
       </c>
       <c r="R9">
-        <f>O9+P9+Q9</f>
+        <f t="shared" si="0"/>
         <v>3.65</v>
       </c>
-      <c r="S9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1227,14 +1203,11 @@
         <v>3.84</v>
       </c>
       <c r="R10">
-        <f>O10+P10+Q10</f>
+        <f t="shared" si="0"/>
         <v>3.84</v>
       </c>
-      <c r="S10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>12</v>
       </c>
@@ -1281,14 +1254,11 @@
         <v>3.84</v>
       </c>
       <c r="R11">
-        <f>O11+P11+Q11</f>
+        <f t="shared" si="0"/>
         <v>3.84</v>
       </c>
-      <c r="S11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>53</v>
       </c>
@@ -1338,11 +1308,11 @@
         <v>3.44</v>
       </c>
       <c r="R12">
-        <f>O12+P12+Q12</f>
+        <f t="shared" si="0"/>
         <v>5.88</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -1392,11 +1362,11 @@
         <v>4.42</v>
       </c>
       <c r="R13">
-        <f>O13+P13+Q13</f>
+        <f t="shared" si="0"/>
         <v>6.7799999999999994</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>18</v>
       </c>
@@ -1443,14 +1413,11 @@
         <v>8</v>
       </c>
       <c r="R14">
-        <f>O14+P14+Q14</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="S14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>29</v>
       </c>
@@ -1500,11 +1467,11 @@
         <v>5.0199999999999996</v>
       </c>
       <c r="R15">
-        <f>O15+P15+Q15</f>
+        <f t="shared" si="0"/>
         <v>8.18</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>22</v>
       </c>
@@ -1551,11 +1518,11 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="R16">
-        <f>O16+P16+Q16</f>
+        <f t="shared" si="0"/>
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>69</v>
       </c>
@@ -1605,11 +1572,11 @@
         <v>2.84</v>
       </c>
       <c r="R17">
-        <f>O17+P17+Q17</f>
+        <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>40</v>
       </c>
@@ -1659,11 +1626,11 @@
         <v>0.9</v>
       </c>
       <c r="R18">
-        <f>O18+P18+Q18</f>
+        <f t="shared" si="0"/>
         <v>7.2600000000000007</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>25</v>
       </c>
@@ -1713,11 +1680,11 @@
         <v>1.57</v>
       </c>
       <c r="R19">
-        <f>O19+P19+Q19</f>
+        <f t="shared" si="0"/>
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>56</v>
       </c>
@@ -1767,11 +1734,11 @@
         <v>9.14</v>
       </c>
       <c r="R20">
-        <f>O20+P20+Q20</f>
+        <f t="shared" si="0"/>
         <v>12.34</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>42</v>
       </c>
@@ -1821,11 +1788,11 @@
         <v>11.53</v>
       </c>
       <c r="R21">
-        <f>O21+P21+Q21</f>
+        <f t="shared" si="0"/>
         <v>15.459999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>31</v>
       </c>
@@ -1875,11 +1842,11 @@
         <v>11.89</v>
       </c>
       <c r="R22">
-        <f>O22+P22+Q22</f>
+        <f t="shared" si="0"/>
         <v>15.75</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>52</v>
       </c>
@@ -1926,14 +1893,11 @@
         <v>1.67</v>
       </c>
       <c r="R23">
-        <f>O23+P23+Q23</f>
+        <f t="shared" si="0"/>
         <v>1.67</v>
       </c>
-      <c r="S23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2</v>
       </c>
@@ -1980,11 +1944,11 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="R24">
-        <f>O24+P24+Q24</f>
+        <f t="shared" si="0"/>
         <v>2.2400000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>43</v>
       </c>
@@ -2031,11 +1995,11 @@
         <v>2.76</v>
       </c>
       <c r="R25">
-        <f>O25+P25+Q25</f>
+        <f t="shared" si="0"/>
         <v>2.76</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>4</v>
       </c>
@@ -2082,11 +2046,11 @@
         <v>3.39</v>
       </c>
       <c r="R26">
-        <f>O26+P26+Q26</f>
+        <f t="shared" si="0"/>
         <v>3.39</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -2136,11 +2100,11 @@
         <v>3.42</v>
       </c>
       <c r="R27">
-        <f>O27+P27+Q27</f>
+        <f t="shared" si="0"/>
         <v>6.71</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>21</v>
       </c>
@@ -2187,11 +2151,11 @@
         <v>16.25</v>
       </c>
       <c r="R28">
-        <f>O28+P28+Q28</f>
+        <f t="shared" si="0"/>
         <v>16.25</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>44</v>
       </c>
@@ -2235,11 +2199,11 @@
         <v>3.77</v>
       </c>
       <c r="R29">
-        <f>O29+P29+Q29</f>
+        <f t="shared" si="0"/>
         <v>3.77</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>32</v>
       </c>
@@ -2286,11 +2250,11 @@
         <v>4.8899999999999997</v>
       </c>
       <c r="R30">
-        <f>O30+P30+Q30</f>
+        <f t="shared" si="0"/>
         <v>4.8899999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>20</v>
       </c>
@@ -2340,11 +2304,11 @@
         <v>5.86</v>
       </c>
       <c r="R31">
-        <f>O31+P31+Q31</f>
+        <f t="shared" si="0"/>
         <v>11.57</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>0</v>
       </c>
@@ -2388,7 +2352,7 @@
         <v>2</v>
       </c>
       <c r="R32">
-        <f>O32+P32+Q32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2436,7 +2400,7 @@
         <v>2</v>
       </c>
       <c r="R33">
-        <f>O33+P33+Q33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2487,7 +2451,7 @@
         <v>3.16</v>
       </c>
       <c r="R34">
-        <f>O34+P34+Q34</f>
+        <f t="shared" ref="R34:R65" si="1">O34+P34+Q34</f>
         <v>3.16</v>
       </c>
     </row>
@@ -2538,7 +2502,7 @@
         <v>3.42</v>
       </c>
       <c r="R35">
-        <f>O35+P35+Q35</f>
+        <f t="shared" si="1"/>
         <v>3.42</v>
       </c>
     </row>
@@ -2592,7 +2556,7 @@
         <v>2.42</v>
       </c>
       <c r="R36">
-        <f>O36+P36+Q36</f>
+        <f t="shared" si="1"/>
         <v>4.1500000000000004</v>
       </c>
     </row>
@@ -2646,7 +2610,7 @@
         <v>3.34</v>
       </c>
       <c r="R37">
-        <f>O37+P37+Q37</f>
+        <f t="shared" si="1"/>
         <v>6.01</v>
       </c>
     </row>
@@ -2700,7 +2664,7 @@
         <v>1.57</v>
       </c>
       <c r="R38">
-        <f>O38+P38+Q38</f>
+        <f t="shared" si="1"/>
         <v>9.3000000000000007</v>
       </c>
     </row>
@@ -2754,7 +2718,7 @@
         <v>8.18</v>
       </c>
       <c r="R39">
-        <f>O39+P39+Q39</f>
+        <f t="shared" si="1"/>
         <v>10.08</v>
       </c>
     </row>
@@ -2808,7 +2772,7 @@
         <v>8.14</v>
       </c>
       <c r="R40">
-        <f>O40+P40+Q40</f>
+        <f t="shared" si="1"/>
         <v>10.42</v>
       </c>
     </row>
@@ -2859,7 +2823,7 @@
         <v>10.44</v>
       </c>
       <c r="R41">
-        <f>O41+P41+Q41</f>
+        <f t="shared" si="1"/>
         <v>10.44</v>
       </c>
     </row>
@@ -2913,7 +2877,7 @@
         <v>10.75</v>
       </c>
       <c r="R42">
-        <f>O42+P42+Q42</f>
+        <f t="shared" si="1"/>
         <v>13.95</v>
       </c>
     </row>
@@ -2967,7 +2931,7 @@
         <v>12.77</v>
       </c>
       <c r="R43">
-        <f>O43+P43+Q43</f>
+        <f t="shared" si="1"/>
         <v>15.11</v>
       </c>
     </row>
@@ -3021,7 +2985,7 @@
         <v>13.04</v>
       </c>
       <c r="R44">
-        <f>O44+P44+Q44</f>
+        <f t="shared" si="1"/>
         <v>19.619999999999997</v>
       </c>
     </row>
@@ -3075,7 +3039,7 @@
         <v>9.4600000000000009</v>
       </c>
       <c r="R45">
-        <f>O45+P45+Q45</f>
+        <f t="shared" si="1"/>
         <v>20.69</v>
       </c>
     </row>
@@ -3129,7 +3093,7 @@
         <v>11.43</v>
       </c>
       <c r="R46">
-        <f>O46+P46+Q46</f>
+        <f t="shared" si="1"/>
         <v>20.91</v>
       </c>
     </row>
@@ -3186,7 +3150,7 @@
         <v>8.33</v>
       </c>
       <c r="R47">
-        <f>O47+P47+Q47</f>
+        <f t="shared" si="1"/>
         <v>21.02</v>
       </c>
     </row>
@@ -3240,7 +3204,7 @@
         <v>20.14</v>
       </c>
       <c r="R48">
-        <f>O48+P48+Q48</f>
+        <f t="shared" si="1"/>
         <v>22.82</v>
       </c>
     </row>
@@ -3294,7 +3258,7 @@
         <v>19</v>
       </c>
       <c r="R49">
-        <f>O49+P49+Q49</f>
+        <f t="shared" si="1"/>
         <v>22.97</v>
       </c>
     </row>
@@ -3348,7 +3312,7 @@
         <v>21.14</v>
       </c>
       <c r="R50">
-        <f>O50+P50+Q50</f>
+        <f t="shared" si="1"/>
         <v>23.94</v>
       </c>
     </row>
@@ -3402,7 +3366,7 @@
         <v>11.51</v>
       </c>
       <c r="R51">
-        <f>O51+P51+Q51</f>
+        <f t="shared" si="1"/>
         <v>26.41</v>
       </c>
     </row>
@@ -3456,7 +3420,7 @@
         <v>10.210000000000001</v>
       </c>
       <c r="R52">
-        <f>O52+P52+Q52</f>
+        <f t="shared" si="1"/>
         <v>27.16</v>
       </c>
     </row>
@@ -3510,7 +3474,7 @@
         <v>21.04</v>
       </c>
       <c r="R53">
-        <f>O53+P53+Q53</f>
+        <f t="shared" si="1"/>
         <v>32.369999999999997</v>
       </c>
     </row>
@@ -3567,7 +3531,7 @@
         <v>27</v>
       </c>
       <c r="R54">
-        <f>O54+P54+Q54</f>
+        <f t="shared" si="1"/>
         <v>37.269999999999996</v>
       </c>
     </row>
@@ -3624,7 +3588,7 @@
         <v>29.45</v>
       </c>
       <c r="R55">
-        <f>O55+P55+Q55</f>
+        <f t="shared" si="1"/>
         <v>38.79</v>
       </c>
     </row>
@@ -3672,7 +3636,7 @@
         <v>4.17</v>
       </c>
       <c r="R56">
-        <f>O56+P56+Q56</f>
+        <f t="shared" si="1"/>
         <v>4.17</v>
       </c>
     </row>
@@ -3720,7 +3684,7 @@
         <v>4.22</v>
       </c>
       <c r="R57">
-        <f>O57+P57+Q57</f>
+        <f t="shared" si="1"/>
         <v>4.22</v>
       </c>
     </row>
@@ -3768,7 +3732,7 @@
         <v>4.53</v>
       </c>
       <c r="R58">
-        <f>O58+P58+Q58</f>
+        <f t="shared" si="1"/>
         <v>4.53</v>
       </c>
     </row>
@@ -3816,7 +3780,7 @@
         <v>4.55</v>
       </c>
       <c r="R59">
-        <f>O59+P59+Q59</f>
+        <f t="shared" si="1"/>
         <v>4.55</v>
       </c>
     </row>
@@ -3864,7 +3828,7 @@
         <v>6.75</v>
       </c>
       <c r="R60">
-        <f>O60+P60+Q60</f>
+        <f t="shared" si="1"/>
         <v>6.75</v>
       </c>
     </row>
@@ -3912,7 +3876,7 @@
         <v>7.19</v>
       </c>
       <c r="R61">
-        <f>O61+P61+Q61</f>
+        <f t="shared" si="1"/>
         <v>7.19</v>
       </c>
     </row>
@@ -3960,7 +3924,7 @@
         <v>7.26</v>
       </c>
       <c r="R62">
-        <f>O62+P62+Q62</f>
+        <f t="shared" si="1"/>
         <v>7.26</v>
       </c>
     </row>
@@ -4011,7 +3975,7 @@
         <v>5.67</v>
       </c>
       <c r="R63">
-        <f>O63+P63+Q63</f>
+        <f t="shared" si="1"/>
         <v>7.6899999999999995</v>
       </c>
     </row>
@@ -4059,7 +4023,7 @@
         <v>7.94</v>
       </c>
       <c r="R64">
-        <f>O64+P64+Q64</f>
+        <f t="shared" si="1"/>
         <v>7.94</v>
       </c>
     </row>
@@ -4110,7 +4074,7 @@
         <v>9.7200000000000006</v>
       </c>
       <c r="R65">
-        <f>O65+P65+Q65</f>
+        <f t="shared" si="1"/>
         <v>10.57</v>
       </c>
     </row>
@@ -4161,7 +4125,7 @@
         <v>9.0500000000000007</v>
       </c>
       <c r="R66">
-        <f>O66+P66+Q66</f>
+        <f t="shared" ref="R66:R97" si="2">O66+P66+Q66</f>
         <v>11.370000000000001</v>
       </c>
     </row>
@@ -4209,7 +4173,7 @@
         <v>14.95</v>
       </c>
       <c r="R67">
-        <f>O67+P67+Q67</f>
+        <f t="shared" si="2"/>
         <v>14.95</v>
       </c>
     </row>
@@ -4260,12 +4224,12 @@
         <v>25.49</v>
       </c>
       <c r="R68">
-        <f>O68+P68+Q68</f>
+        <f t="shared" si="2"/>
         <v>32.72</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:S68">
+  <sortState ref="A2:R68">
     <sortCondition descending="1" ref="N1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4281,6 +4245,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068154D9CED6A274799344D73CDDB6092" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5a2665e4f307efafdee1c9405c7148c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0" xmlns:ns4="a05e4abd-8455-4909-9372-067b8b6e3dbc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb69d6d218e7dc1efa9607e3a9562cb6" ns3:_="" ns4:_="">
     <xsd:import namespace="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
@@ -4489,33 +4462,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FD1C522-C9EE-4918-8E62-07B8615331B6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="a05e4abd-8455-4909-9372-067b8b6e3dbc"/>
     <ds:schemaRef ds:uri="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1224F8E3-B117-4CC1-A01B-C7E870A3F236}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEEE5A80-C520-49F1-8D68-0739C0E45C24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4532,12 +4504,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1224F8E3-B117-4CC1-A01B-C7E870A3F236}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>